<commit_message>
Update README, add media
</commit_message>
<xml_diff>
--- a/inputs/input.xlsx
+++ b/inputs/input.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>sample_id</t>
   </si>
@@ -22,19 +22,34 @@
     <t>lon</t>
   </si>
   <si>
-    <t>R001</t>
-  </si>
-  <si>
-    <t>R002</t>
-  </si>
-  <si>
-    <t>R003</t>
-  </si>
-  <si>
-    <t>R004</t>
-  </si>
-  <si>
-    <t>R005</t>
+    <t>BLT_001</t>
+  </si>
+  <si>
+    <t>BLR_002</t>
+  </si>
+  <si>
+    <t>MYS_001</t>
+  </si>
+  <si>
+    <t>RUR_001</t>
+  </si>
+  <si>
+    <t>DEL_001</t>
+  </si>
+  <si>
+    <t>MUM_001</t>
+  </si>
+  <si>
+    <t>PUN_001</t>
+  </si>
+  <si>
+    <t>HYD_001</t>
+  </si>
+  <si>
+    <t>VHN-001</t>
+  </si>
+  <si>
+    <t>AGRI_001</t>
   </si>
 </sst>
 </file>
@@ -318,10 +333,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>28.6139</v>
+        <v>12.9352</v>
       </c>
       <c r="C3" s="1">
-        <v>77.209</v>
+        <v>77.6146</v>
       </c>
     </row>
     <row r="4">
@@ -329,10 +344,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>19.076</v>
+        <v>12.2958</v>
       </c>
       <c r="C4" s="1">
-        <v>72.8777</v>
+        <v>76.6394</v>
       </c>
     </row>
     <row r="5">
@@ -340,10 +355,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>13.0827</v>
+        <v>13.3392</v>
       </c>
       <c r="C5" s="1">
-        <v>80.2707</v>
+        <v>77.1135</v>
       </c>
     </row>
     <row r="6">
@@ -351,10 +366,65 @@
         <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>22.5726</v>
+        <v>28.6139</v>
       </c>
       <c r="C6" s="1">
-        <v>88.3639</v>
+        <v>77.209</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>19.076</v>
+      </c>
+      <c r="C7" s="1">
+        <v>72.8777</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>18.5204</v>
+      </c>
+      <c r="C8" s="1">
+        <v>73.8567</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>17.385</v>
+      </c>
+      <c r="C9" s="1">
+        <v>78.4867</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>13.0827</v>
+      </c>
+      <c r="C10" s="1">
+        <v>80.2707</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>11.1271</v>
+      </c>
+      <c r="C11" s="1">
+        <v>78.6569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>